<commit_message>
Add Types, DataAnalyzer, Part of parsing
</commit_message>
<xml_diff>
--- a/docs/table.xlsx
+++ b/docs/table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3E0A46-0A79-482D-9BBC-65286AC1E9C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA08FC2-16BA-4AE8-95FD-7853BD59DDCF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="40">
   <si>
     <t>if</t>
   </si>
@@ -67,9 +67,6 @@
     <t>)</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>bool</t>
   </si>
   <si>
@@ -133,12 +130,6 @@
     <t>.</t>
   </si>
   <si>
-    <t xml:space="preserve">    '</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  '</t>
-  </si>
-  <si>
     <t>[0-9] и [A-z] - константы или индификаторы, нужно определять, правило указывает, что следущий литерал начинается с цифры или буквы</t>
   </si>
   <si>
@@ -146,13 +137,22 @@
   </si>
   <si>
     <t>return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> `</t>
+  </si>
+  <si>
+    <t>cin/out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +177,24 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +224,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -466,11 +492,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -555,9 +583,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="18" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
     <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -839,20 +888,20 @@
   <dimension ref="A1:AK42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>0</v>
@@ -872,11 +921,11 @@
       <c r="I1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="40" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L1" s="19" t="s">
         <v>7</v>
@@ -884,10 +933,10 @@
       <c r="M1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="40" t="s">
         <v>10</v>
       </c>
       <c r="P1" s="19" t="s">
@@ -896,70 +945,70 @@
       <c r="Q1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="19" t="s">
-        <v>13</v>
+      <c r="R1" s="47" t="s">
+        <v>39</v>
       </c>
       <c r="S1" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Z1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="AA1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="20" t="s">
+      <c r="AB1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="20" t="s">
-        <v>24</v>
-      </c>
       <c r="AC1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="20" t="s">
+      <c r="AE1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="20" t="s">
+      <c r="AF1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="20" t="s">
+      <c r="AG1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="20" t="s">
+      <c r="AH1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="AI1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="11"/>
@@ -969,7 +1018,7 @@
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="J2" s="41"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="37">
@@ -999,7 +1048,7 @@
       <c r="W2" s="37">
         <v>8</v>
       </c>
-      <c r="X2" s="37">
+      <c r="X2" s="41">
         <v>9</v>
       </c>
       <c r="Y2" s="37">
@@ -1032,7 +1081,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="22"/>
@@ -1042,7 +1091,7 @@
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
+      <c r="J3" s="42"/>
       <c r="K3" s="22"/>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
@@ -1068,7 +1117,7 @@
       <c r="W3" s="14">
         <v>6</v>
       </c>
-      <c r="X3" s="14">
+      <c r="X3" s="42">
         <v>7</v>
       </c>
       <c r="Y3" s="22"/>
@@ -1103,7 +1152,7 @@
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
+      <c r="J4" s="42"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
@@ -1119,7 +1168,7 @@
       <c r="U4" s="13"/>
       <c r="V4" s="13"/>
       <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
+      <c r="X4" s="42"/>
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
       <c r="AA4" s="13"/>
@@ -1150,7 +1199,7 @@
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
@@ -1166,7 +1215,7 @@
       <c r="U5" s="22"/>
       <c r="V5" s="22"/>
       <c r="W5" s="22"/>
-      <c r="X5" s="22"/>
+      <c r="X5" s="42"/>
       <c r="Y5" s="22"/>
       <c r="Z5" s="22"/>
       <c r="AA5" s="22"/>
@@ -1195,7 +1244,7 @@
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="J6" s="42"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -1211,7 +1260,7 @@
       <c r="U6" s="13"/>
       <c r="V6" s="13"/>
       <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
+      <c r="X6" s="42"/>
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
       <c r="AA6" s="13"/>
@@ -1240,7 +1289,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="J7" s="42"/>
       <c r="K7" s="22"/>
       <c r="L7" s="14">
         <v>2</v>
@@ -1256,7 +1305,7 @@
       <c r="U7" s="22"/>
       <c r="V7" s="22"/>
       <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
+      <c r="X7" s="42"/>
       <c r="Y7" s="22"/>
       <c r="Z7" s="22"/>
       <c r="AA7" s="22"/>
@@ -1287,7 +1336,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+      <c r="J8" s="42"/>
       <c r="K8" s="13"/>
       <c r="L8" s="14">
         <v>2</v>
@@ -1303,7 +1352,7 @@
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
+      <c r="X8" s="42"/>
       <c r="Y8" s="13"/>
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
@@ -1334,7 +1383,7 @@
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
+      <c r="J9" s="42"/>
       <c r="K9" s="22"/>
       <c r="L9" s="14">
         <v>2</v>
@@ -1350,7 +1399,7 @@
       <c r="U9" s="22"/>
       <c r="V9" s="22"/>
       <c r="W9" s="22"/>
-      <c r="X9" s="22"/>
+      <c r="X9" s="42"/>
       <c r="Y9" s="22"/>
       <c r="Z9" s="22"/>
       <c r="AA9" s="22"/>
@@ -1368,55 +1417,55 @@
       <c r="AK9" s="29"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="14">
+      <c r="B10" s="45"/>
+      <c r="C10" s="42">
         <v>1</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="14">
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42">
         <v>2</v>
       </c>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="14">
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="42"/>
+      <c r="V10" s="42"/>
+      <c r="W10" s="42"/>
+      <c r="X10" s="42"/>
+      <c r="Y10" s="42"/>
+      <c r="Z10" s="42"/>
+      <c r="AA10" s="42"/>
+      <c r="AB10" s="42"/>
+      <c r="AC10" s="42"/>
+      <c r="AD10" s="42"/>
+      <c r="AE10" s="42">
         <v>3</v>
       </c>
-      <c r="AF10" s="30"/>
-      <c r="AG10" s="30"/>
-      <c r="AH10" s="30"/>
-      <c r="AI10" s="30"/>
-      <c r="AJ10" s="30"/>
-      <c r="AK10" s="31"/>
+      <c r="AF10" s="42"/>
+      <c r="AG10" s="42"/>
+      <c r="AH10" s="42"/>
+      <c r="AI10" s="42"/>
+      <c r="AJ10" s="42"/>
+      <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="14">
@@ -1428,7 +1477,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="J11" s="42"/>
       <c r="K11" s="22"/>
       <c r="L11" s="14">
         <v>2</v>
@@ -1444,7 +1493,7 @@
       <c r="U11" s="22"/>
       <c r="V11" s="22"/>
       <c r="W11" s="22"/>
-      <c r="X11" s="22"/>
+      <c r="X11" s="42"/>
       <c r="Y11" s="22"/>
       <c r="Z11" s="22"/>
       <c r="AA11" s="22"/>
@@ -1475,7 +1524,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="J12" s="42"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="14">
@@ -1491,7 +1540,7 @@
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
       <c r="W12" s="13"/>
-      <c r="X12" s="14">
+      <c r="X12" s="42">
         <v>3</v>
       </c>
       <c r="Y12" s="13"/>
@@ -1526,7 +1575,7 @@
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="J13" s="42"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
@@ -1544,7 +1593,7 @@
       <c r="W13" s="14">
         <v>3</v>
       </c>
-      <c r="X13" s="22"/>
+      <c r="X13" s="42"/>
       <c r="Y13" s="22"/>
       <c r="Z13" s="22"/>
       <c r="AA13" s="22"/>
@@ -1562,7 +1611,7 @@
       <c r="AK13" s="29"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="24">
@@ -1587,7 +1636,7 @@
       <c r="I14" s="14">
         <v>7</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="42">
         <v>8</v>
       </c>
       <c r="K14" s="14">
@@ -1609,7 +1658,7 @@
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
       <c r="W14" s="13"/>
-      <c r="X14" s="14">
+      <c r="X14" s="42">
         <v>11</v>
       </c>
       <c r="Y14" s="13"/>
@@ -1635,7 +1684,7 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="44" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="21"/>
@@ -1660,7 +1709,7 @@
       <c r="I15" s="14">
         <v>8</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="42">
         <v>9</v>
       </c>
       <c r="K15" s="14">
@@ -1684,7 +1733,7 @@
       <c r="W15" s="14">
         <v>12</v>
       </c>
-      <c r="X15" s="14">
+      <c r="X15" s="42">
         <v>13</v>
       </c>
       <c r="Y15" s="22"/>
@@ -1725,7 +1774,7 @@
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="J16" s="42"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
@@ -1739,7 +1788,7 @@
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
       <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
+      <c r="X16" s="42"/>
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
       <c r="AA16" s="13"/>
@@ -1766,7 +1815,7 @@
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="J17" s="42"/>
       <c r="K17" s="22"/>
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
@@ -1780,7 +1829,7 @@
       <c r="U17" s="22"/>
       <c r="V17" s="22"/>
       <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
+      <c r="X17" s="42"/>
       <c r="Y17" s="22"/>
       <c r="Z17" s="22"/>
       <c r="AA17" s="22"/>
@@ -1796,8 +1845,8 @@
       <c r="AK17" s="29"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>13</v>
+      <c r="A18" s="48" t="s">
+        <v>39</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -1807,7 +1856,7 @@
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="J18" s="42"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
@@ -1821,7 +1870,7 @@
       <c r="U18" s="13"/>
       <c r="V18" s="13"/>
       <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
+      <c r="X18" s="42"/>
       <c r="Y18" s="13"/>
       <c r="Z18" s="13"/>
       <c r="AA18" s="13"/>
@@ -1838,7 +1887,7 @@
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
@@ -1848,7 +1897,7 @@
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
+      <c r="J19" s="42"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
@@ -1862,7 +1911,7 @@
       <c r="U19" s="22"/>
       <c r="V19" s="22"/>
       <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
+      <c r="X19" s="42"/>
       <c r="Y19" s="22"/>
       <c r="Z19" s="22"/>
       <c r="AA19" s="22"/>
@@ -1879,7 +1928,7 @@
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
@@ -1889,7 +1938,7 @@
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+      <c r="J20" s="42"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
@@ -1903,7 +1952,7 @@
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
       <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
+      <c r="X20" s="42"/>
       <c r="Y20" s="13"/>
       <c r="Z20" s="13"/>
       <c r="AA20" s="13"/>
@@ -1920,7 +1969,7 @@
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
@@ -1930,7 +1979,7 @@
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
+      <c r="J21" s="42"/>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
@@ -1944,7 +1993,7 @@
       <c r="U21" s="22"/>
       <c r="V21" s="22"/>
       <c r="W21" s="22"/>
-      <c r="X21" s="22"/>
+      <c r="X21" s="42"/>
       <c r="Y21" s="22"/>
       <c r="Z21" s="22"/>
       <c r="AA21" s="22"/>
@@ -1961,7 +2010,7 @@
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
@@ -1971,7 +2020,7 @@
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="J22" s="42"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
@@ -1985,7 +2034,7 @@
       <c r="U22" s="13"/>
       <c r="V22" s="13"/>
       <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
+      <c r="X22" s="42"/>
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
       <c r="AA22" s="13"/>
@@ -2002,7 +2051,7 @@
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
@@ -2012,7 +2061,7 @@
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
+      <c r="J23" s="42"/>
       <c r="K23" s="22"/>
       <c r="L23" s="22"/>
       <c r="M23" s="22"/>
@@ -2026,7 +2075,7 @@
       <c r="U23" s="22"/>
       <c r="V23" s="22"/>
       <c r="W23" s="22"/>
-      <c r="X23" s="22"/>
+      <c r="X23" s="42"/>
       <c r="Y23" s="22"/>
       <c r="Z23" s="22"/>
       <c r="AA23" s="22"/>
@@ -2042,49 +2091,49 @@
       <c r="AK23" s="29"/>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
-      <c r="W24" s="13"/>
-      <c r="X24" s="13"/>
-      <c r="Y24" s="13"/>
-      <c r="Z24" s="13"/>
-      <c r="AA24" s="13"/>
-      <c r="AB24" s="13"/>
-      <c r="AC24" s="13"/>
-      <c r="AD24" s="13"/>
-      <c r="AE24" s="13"/>
-      <c r="AF24" s="30"/>
-      <c r="AG24" s="30"/>
-      <c r="AH24" s="30"/>
-      <c r="AI24" s="30"/>
-      <c r="AJ24" s="30"/>
-      <c r="AK24" s="31"/>
+      <c r="A24" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="45"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="42"/>
+      <c r="U24" s="42"/>
+      <c r="V24" s="42"/>
+      <c r="W24" s="42"/>
+      <c r="X24" s="42"/>
+      <c r="Y24" s="42"/>
+      <c r="Z24" s="42"/>
+      <c r="AA24" s="42"/>
+      <c r="AB24" s="42"/>
+      <c r="AC24" s="42"/>
+      <c r="AD24" s="42"/>
+      <c r="AE24" s="42"/>
+      <c r="AF24" s="42"/>
+      <c r="AG24" s="42"/>
+      <c r="AH24" s="42"/>
+      <c r="AI24" s="42"/>
+      <c r="AJ24" s="42"/>
+      <c r="AK24" s="46"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
@@ -2094,7 +2143,7 @@
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
+      <c r="J25" s="42"/>
       <c r="K25" s="22"/>
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
@@ -2108,7 +2157,7 @@
       <c r="U25" s="22"/>
       <c r="V25" s="22"/>
       <c r="W25" s="22"/>
-      <c r="X25" s="22"/>
+      <c r="X25" s="42"/>
       <c r="Y25" s="22"/>
       <c r="Z25" s="22"/>
       <c r="AA25" s="22"/>
@@ -2125,7 +2174,7 @@
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
@@ -2135,7 +2184,7 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
+      <c r="J26" s="42"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
@@ -2149,7 +2198,7 @@
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
       <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
+      <c r="X26" s="42"/>
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
       <c r="AA26" s="13"/>
@@ -2166,7 +2215,7 @@
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
@@ -2176,7 +2225,7 @@
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="J27" s="42"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
       <c r="M27" s="22"/>
@@ -2190,7 +2239,7 @@
       <c r="U27" s="22"/>
       <c r="V27" s="22"/>
       <c r="W27" s="22"/>
-      <c r="X27" s="22"/>
+      <c r="X27" s="42"/>
       <c r="Y27" s="22"/>
       <c r="Z27" s="22"/>
       <c r="AA27" s="22"/>
@@ -2207,7 +2256,7 @@
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
@@ -2217,7 +2266,7 @@
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
+      <c r="J28" s="42"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
@@ -2231,7 +2280,7 @@
       <c r="U28" s="13"/>
       <c r="V28" s="13"/>
       <c r="W28" s="13"/>
-      <c r="X28" s="13"/>
+      <c r="X28" s="42"/>
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
       <c r="AA28" s="13"/>
@@ -2248,7 +2297,7 @@
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
@@ -2258,7 +2307,7 @@
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
+      <c r="J29" s="42"/>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
       <c r="M29" s="22"/>
@@ -2272,7 +2321,7 @@
       <c r="U29" s="22"/>
       <c r="V29" s="22"/>
       <c r="W29" s="22"/>
-      <c r="X29" s="22"/>
+      <c r="X29" s="42"/>
       <c r="Y29" s="22"/>
       <c r="Z29" s="22"/>
       <c r="AA29" s="22"/>
@@ -2289,7 +2338,7 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
@@ -2299,7 +2348,7 @@
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
+      <c r="J30" s="42"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
@@ -2313,7 +2362,7 @@
       <c r="U30" s="13"/>
       <c r="V30" s="13"/>
       <c r="W30" s="13"/>
-      <c r="X30" s="13"/>
+      <c r="X30" s="42"/>
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
       <c r="AA30" s="13"/>
@@ -2330,7 +2379,7 @@
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
@@ -2340,7 +2389,7 @@
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
+      <c r="J31" s="42"/>
       <c r="K31" s="22"/>
       <c r="L31" s="22"/>
       <c r="M31" s="22"/>
@@ -2354,7 +2403,7 @@
       <c r="U31" s="22"/>
       <c r="V31" s="22"/>
       <c r="W31" s="22"/>
-      <c r="X31" s="22"/>
+      <c r="X31" s="42"/>
       <c r="Y31" s="22"/>
       <c r="Z31" s="22"/>
       <c r="AA31" s="22"/>
@@ -2371,7 +2420,7 @@
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="32"/>
       <c r="C32" s="30"/>
@@ -2381,7 +2430,7 @@
       <c r="G32" s="30"/>
       <c r="H32" s="30"/>
       <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
+      <c r="J32" s="42"/>
       <c r="K32" s="30"/>
       <c r="L32" s="30"/>
       <c r="M32" s="30"/>
@@ -2395,7 +2444,7 @@
       <c r="U32" s="30"/>
       <c r="V32" s="30"/>
       <c r="W32" s="30"/>
-      <c r="X32" s="30"/>
+      <c r="X32" s="42"/>
       <c r="Y32" s="30"/>
       <c r="Z32" s="30"/>
       <c r="AA32" s="30"/>
@@ -2412,7 +2461,7 @@
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="33"/>
       <c r="C33" s="28"/>
@@ -2422,7 +2471,7 @@
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
+      <c r="J33" s="42"/>
       <c r="K33" s="28"/>
       <c r="L33" s="28"/>
       <c r="M33" s="28"/>
@@ -2436,7 +2485,7 @@
       <c r="U33" s="28"/>
       <c r="V33" s="28"/>
       <c r="W33" s="28"/>
-      <c r="X33" s="28"/>
+      <c r="X33" s="42"/>
       <c r="Y33" s="28"/>
       <c r="Z33" s="28"/>
       <c r="AA33" s="28"/>
@@ -2453,7 +2502,7 @@
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="32"/>
       <c r="C34" s="30"/>
@@ -2463,7 +2512,7 @@
       <c r="G34" s="30"/>
       <c r="H34" s="30"/>
       <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
+      <c r="J34" s="42"/>
       <c r="K34" s="30"/>
       <c r="L34" s="30"/>
       <c r="M34" s="30"/>
@@ -2477,7 +2526,7 @@
       <c r="U34" s="30"/>
       <c r="V34" s="30"/>
       <c r="W34" s="30"/>
-      <c r="X34" s="30"/>
+      <c r="X34" s="42"/>
       <c r="Y34" s="30"/>
       <c r="Z34" s="30"/>
       <c r="AA34" s="30"/>
@@ -2494,7 +2543,7 @@
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="38" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="28"/>
@@ -2504,7 +2553,7 @@
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
+      <c r="J35" s="42"/>
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
       <c r="M35" s="28"/>
@@ -2518,7 +2567,7 @@
       <c r="U35" s="28"/>
       <c r="V35" s="28"/>
       <c r="W35" s="28"/>
-      <c r="X35" s="28"/>
+      <c r="X35" s="42"/>
       <c r="Y35" s="28"/>
       <c r="Z35" s="28"/>
       <c r="AA35" s="28"/>
@@ -2535,7 +2584,7 @@
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" s="32"/>
       <c r="C36" s="30"/>
@@ -2545,7 +2594,7 @@
       <c r="G36" s="30"/>
       <c r="H36" s="30"/>
       <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
+      <c r="J36" s="42"/>
       <c r="K36" s="30"/>
       <c r="L36" s="30"/>
       <c r="M36" s="30"/>
@@ -2559,7 +2608,7 @@
       <c r="U36" s="30"/>
       <c r="V36" s="30"/>
       <c r="W36" s="30"/>
-      <c r="X36" s="30"/>
+      <c r="X36" s="42"/>
       <c r="Y36" s="30"/>
       <c r="Z36" s="30"/>
       <c r="AA36" s="30"/>
@@ -2576,7 +2625,7 @@
     </row>
     <row r="37" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="39" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B37" s="34"/>
       <c r="C37" s="35"/>
@@ -2586,7 +2635,7 @@
       <c r="G37" s="35"/>
       <c r="H37" s="35"/>
       <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="J37" s="43"/>
       <c r="K37" s="35"/>
       <c r="L37" s="35"/>
       <c r="M37" s="35"/>
@@ -2600,7 +2649,7 @@
       <c r="U37" s="35"/>
       <c r="V37" s="35"/>
       <c r="W37" s="35"/>
-      <c r="X37" s="35"/>
+      <c r="X37" s="43"/>
       <c r="Y37" s="35"/>
       <c r="Z37" s="35"/>
       <c r="AA37" s="35"/>
@@ -2617,12 +2666,12 @@
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>

</xml_diff>

<commit_message>
Add Limiters, +new const
</commit_message>
<xml_diff>
--- a/docs/table.xlsx
+++ b/docs/table.xlsx
@@ -467,7 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -542,9 +542,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -866,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="K4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,7 +998,7 @@
       <c r="N2" s="21"/>
       <c r="O2" s="20"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="50"/>
+      <c r="Q2" s="49"/>
       <c r="R2" s="20"/>
       <c r="S2" s="21"/>
       <c r="T2" s="21"/>
@@ -1254,7 +1251,6 @@
       <c r="AA8" s="31"/>
       <c r="AB8" s="31"/>
       <c r="AC8" s="31"/>
-      <c r="AD8" s="38"/>
       <c r="AE8" s="33"/>
       <c r="AF8" s="33"/>
       <c r="AG8" s="33"/>
@@ -1306,47 +1302,47 @@
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="36"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
       <c r="K10" s="36"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="40"/>
-      <c r="T10" s="40"/>
-      <c r="U10" s="40"/>
-      <c r="V10" s="40"/>
-      <c r="W10" s="40"/>
-      <c r="X10" s="40"/>
-      <c r="Y10" s="40"/>
-      <c r="Z10" s="40"/>
-      <c r="AA10" s="40"/>
-      <c r="AB10" s="40"/>
-      <c r="AC10" s="40"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="39"/>
+      <c r="T10" s="39"/>
+      <c r="U10" s="39"/>
+      <c r="V10" s="39"/>
+      <c r="W10" s="39"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="39"/>
+      <c r="Z10" s="39"/>
+      <c r="AA10" s="39"/>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="39"/>
       <c r="AD10" s="36"/>
-      <c r="AE10" s="41"/>
-      <c r="AF10" s="41"/>
-      <c r="AG10" s="41"/>
-      <c r="AH10" s="41"/>
-      <c r="AI10" s="41"/>
-      <c r="AJ10" s="42"/>
+      <c r="AE10" s="40"/>
+      <c r="AF10" s="40"/>
+      <c r="AG10" s="40"/>
+      <c r="AH10" s="40"/>
+      <c r="AI10" s="40"/>
+      <c r="AJ10" s="41"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="43"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -1386,47 +1382,47 @@
       <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="39"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="36"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
       <c r="M12" s="36"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="40"/>
-      <c r="T12" s="40"/>
-      <c r="U12" s="40"/>
-      <c r="V12" s="40"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="39"/>
       <c r="W12" s="36"/>
-      <c r="X12" s="40"/>
-      <c r="Y12" s="40"/>
-      <c r="Z12" s="40"/>
-      <c r="AA12" s="40"/>
-      <c r="AB12" s="40"/>
-      <c r="AC12" s="40"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="39"/>
+      <c r="Z12" s="39"/>
+      <c r="AA12" s="39"/>
+      <c r="AB12" s="39"/>
+      <c r="AC12" s="39"/>
       <c r="AD12" s="36"/>
-      <c r="AE12" s="41"/>
-      <c r="AF12" s="41"/>
-      <c r="AG12" s="41"/>
-      <c r="AH12" s="41"/>
-      <c r="AI12" s="41"/>
-      <c r="AJ12" s="42"/>
+      <c r="AE12" s="40"/>
+      <c r="AF12" s="40"/>
+      <c r="AG12" s="40"/>
+      <c r="AH12" s="40"/>
+      <c r="AI12" s="40"/>
+      <c r="AJ12" s="41"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="43"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
       <c r="E13" s="26"/>
@@ -1466,7 +1462,7 @@
       <c r="A14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="39"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
@@ -1475,32 +1471,32 @@
       <c r="H14" s="36"/>
       <c r="I14" s="36"/>
       <c r="J14" s="36"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
       <c r="M14" s="36"/>
       <c r="N14" s="36"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="40"/>
-      <c r="T14" s="40"/>
-      <c r="U14" s="40"/>
-      <c r="V14" s="40"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="39"/>
       <c r="W14" s="36"/>
-      <c r="X14" s="40"/>
-      <c r="Y14" s="40"/>
-      <c r="Z14" s="40"/>
-      <c r="AA14" s="40"/>
-      <c r="AB14" s="40"/>
-      <c r="AC14" s="40"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="39"/>
       <c r="AD14" s="36"/>
       <c r="AE14" s="36"/>
       <c r="AF14" s="36"/>
-      <c r="AG14" s="41"/>
+      <c r="AG14" s="40"/>
       <c r="AH14" s="36"/>
       <c r="AI14" s="36"/>
-      <c r="AJ14" s="44"/>
+      <c r="AJ14" s="43"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1546,47 +1542,47 @@
       <c r="A16" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="40"/>
-      <c r="S16" s="40"/>
-      <c r="T16" s="40"/>
-      <c r="U16" s="40"/>
-      <c r="V16" s="40"/>
-      <c r="W16" s="40"/>
-      <c r="X16" s="40"/>
-      <c r="Y16" s="40"/>
-      <c r="Z16" s="40"/>
-      <c r="AA16" s="40"/>
-      <c r="AB16" s="40"/>
-      <c r="AC16" s="40"/>
-      <c r="AD16" s="40"/>
-      <c r="AE16" s="41"/>
-      <c r="AF16" s="41"/>
-      <c r="AG16" s="41"/>
-      <c r="AH16" s="41"/>
-      <c r="AI16" s="41"/>
-      <c r="AJ16" s="42"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39"/>
+      <c r="Z16" s="39"/>
+      <c r="AA16" s="39"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="39"/>
+      <c r="AD16" s="39"/>
+      <c r="AE16" s="40"/>
+      <c r="AF16" s="40"/>
+      <c r="AG16" s="40"/>
+      <c r="AH16" s="40"/>
+      <c r="AI16" s="40"/>
+      <c r="AJ16" s="41"/>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="46"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
@@ -2146,7 +2142,7 @@
       <c r="A31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="45"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
@@ -2186,7 +2182,7 @@
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="46"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
@@ -2226,7 +2222,7 @@
       <c r="A33" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="45"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
@@ -2266,7 +2262,7 @@
       <c r="A34" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="46"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="28"/>
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
@@ -2306,7 +2302,7 @@
       <c r="A35" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="45"/>
+      <c r="B35" s="44"/>
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
       <c r="E35" s="33"/>
@@ -2346,41 +2342,41 @@
       <c r="A36" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="O36" s="48"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
-      <c r="R36" s="48"/>
-      <c r="S36" s="48"/>
-      <c r="T36" s="48"/>
-      <c r="U36" s="48"/>
-      <c r="V36" s="48"/>
-      <c r="W36" s="48"/>
-      <c r="X36" s="48"/>
-      <c r="Y36" s="48"/>
-      <c r="Z36" s="48"/>
-      <c r="AA36" s="48"/>
-      <c r="AB36" s="48"/>
-      <c r="AC36" s="48"/>
-      <c r="AD36" s="48"/>
-      <c r="AE36" s="48"/>
-      <c r="AF36" s="48"/>
-      <c r="AG36" s="48"/>
-      <c r="AH36" s="48"/>
-      <c r="AI36" s="48"/>
-      <c r="AJ36" s="49"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="47"/>
+      <c r="R36" s="47"/>
+      <c r="S36" s="47"/>
+      <c r="T36" s="47"/>
+      <c r="U36" s="47"/>
+      <c r="V36" s="47"/>
+      <c r="W36" s="47"/>
+      <c r="X36" s="47"/>
+      <c r="Y36" s="47"/>
+      <c r="Z36" s="47"/>
+      <c r="AA36" s="47"/>
+      <c r="AB36" s="47"/>
+      <c r="AC36" s="47"/>
+      <c r="AD36" s="47"/>
+      <c r="AE36" s="47"/>
+      <c r="AF36" s="47"/>
+      <c r="AG36" s="47"/>
+      <c r="AH36" s="47"/>
+      <c r="AI36" s="47"/>
+      <c r="AJ36" s="48"/>
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" t="s">

</xml_diff>

<commit_message>
Fix error with tabulation
</commit_message>
<xml_diff>
--- a/docs/table.xlsx
+++ b/docs/table.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C897DBE-A2EE-42E8-9303-4064E470FD9A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -189,7 +190,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -674,11 +675,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW4" sqref="AW4"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,17 +877,11 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4">
-        <v>10</v>
-      </c>
+      <c r="O3" s="4"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="4">
-        <v>10</v>
-      </c>
+      <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="4">
-        <v>10</v>
-      </c>
+      <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>

</xml_diff>

<commit_message>
Add some test. Rework Lexer logic
</commit_message>
<xml_diff>
--- a/docs/table.xlsx
+++ b/docs/table.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8F63D7-F379-4411-BF40-E09653AFA4AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2655" yWindow="2685" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="66">
   <si>
     <t>s</t>
   </si>
@@ -215,12 +214,15 @@
   </si>
   <si>
     <t>=&gt; косяк с пробелом поправить для string</t>
+  </si>
+  <si>
+    <t>//переделать</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -723,11 +725,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL25" sqref="AL25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR13" sqref="AR13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,7 +1509,9 @@
       <c r="AF13" s="8"/>
       <c r="AG13" s="8"/>
       <c r="AH13" s="8"/>
-      <c r="AI13" s="8"/>
+      <c r="AI13" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="AJ13" s="8"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
@@ -1675,6 +1679,9 @@
       <c r="AE15" s="8"/>
       <c r="AF15" s="13"/>
       <c r="AG15" s="13"/>
+      <c r="AI15" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">

</xml_diff>